<commit_message>
Started the PCBnew and added IRF3205 to BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard.xlsx
+++ b/BOM/BOM_PowerBoard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\codyb\USST\rover-hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B5A8ED-B54F-2B4D-823E-F7496313C3F4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD3D288-DEA7-4325-8F69-321CF6A656D3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14060" yWindow="460" windowWidth="10080" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
   <si>
     <t>Manufacturer Number</t>
   </si>
@@ -238,13 +238,19 @@
   </si>
   <si>
     <t>Wurth Electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infineon Technologies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRF3205PBF 110A TO-220AB Package </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -282,6 +288,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -303,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -311,6 +325,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,13 +640,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DE3487-35ED-9947-B91A-5715036B4C63}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
@@ -645,7 +660,7 @@
       </c>
       <c r="B1">
         <f>SUM(G3:G192)</f>
-        <v>88.856380000000016</v>
+        <v>93.076380000000015</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -715,7 +730,7 @@
         <v>2E-3</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G31" si="0">E4*F4</f>
+        <f t="shared" ref="G4:G32" si="0">E4*F4</f>
         <v>2.6000000000000002E-2</v>
       </c>
     </row>
@@ -791,7 +806,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17">
+    <row r="8" spans="1:7" ht="16.5">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -815,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17">
+    <row r="9" spans="1:7" ht="16.5">
       <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
@@ -839,7 +854,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17">
+    <row r="10" spans="1:7" ht="16.5">
       <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
@@ -863,7 +878,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17">
+    <row r="11" spans="1:7" ht="16.5">
       <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
@@ -1079,7 +1094,7 @@
         <v>7.02</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17">
+    <row r="20" spans="1:7" ht="16.5">
       <c r="A20" s="6" t="s">
         <v>45</v>
       </c>
@@ -1367,8 +1382,29 @@
         <v>1.37</v>
       </c>
     </row>
+    <row r="32" spans="1:7">
+      <c r="B32" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="F32" s="4">
+        <v>2.11</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>4.22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
worked on Powerboard PCBnew comments in logbook
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard.xlsx
+++ b/BOM/BOM_PowerBoard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\codyb\USST\rover-hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD3D288-DEA7-4325-8F69-321CF6A656D3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EE07AA-4046-4C35-8FBE-6B25CB004E48}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14060" yWindow="460" windowWidth="10080" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
   <si>
     <t>Manufacturer Number</t>
   </si>
@@ -222,9 +222,6 @@
     <t>ERJ-MP3KF5M0U</t>
   </si>
   <si>
-    <t>5 mOhm 0.5W Resistor</t>
-  </si>
-  <si>
     <t xml:space="preserve">10k Ohm Thermistor </t>
   </si>
   <si>
@@ -244,6 +241,23 @@
   </si>
   <si>
     <t xml:space="preserve">IRF3205PBF 110A TO-220AB Package </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRF3205PBF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MP2060-0.005J-ND </t>
+  </si>
+  <si>
+    <t>Caddock Electronics Inc.</t>
+  </si>
+  <si>
+    <t>5 mOhm 18W Resistor</t>
   </si>
 </sst>
 </file>
@@ -257,11 +271,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <color theme="1"/>
-      <name val="MS"/>
     </font>
     <font>
       <b/>
@@ -278,11 +287,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="HelveticaLTStd"/>
-    </font>
-    <font>
       <sz val="13"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -295,6 +299,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="HelveticaLTStd"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -317,13 +331,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -640,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DE3487-35ED-9947-B91A-5715036B4C63}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -656,11 +676,11 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1">
         <f>SUM(G3:G192)</f>
-        <v>93.076380000000015</v>
+        <v>109.07638000000001</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -683,23 +703,23 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
       <c r="F3">
@@ -711,19 +731,19 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>13</v>
       </c>
       <c r="F4">
@@ -735,19 +755,19 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5">
@@ -759,19 +779,19 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>2</v>
       </c>
       <c r="F6">
@@ -782,20 +802,20 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:7" ht="16.5">
+      <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>18</v>
       </c>
       <c r="F7">
@@ -807,19 +827,19 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.5">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8">
@@ -831,19 +851,19 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.5">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>3</v>
       </c>
       <c r="F9">
@@ -855,19 +875,19 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="16.5">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10">
@@ -879,19 +899,19 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="16.5">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11">
@@ -903,19 +923,19 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>3</v>
       </c>
       <c r="F12">
@@ -930,16 +950,16 @@
       <c r="A13">
         <v>1770539</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>3</v>
       </c>
       <c r="F13">
@@ -954,16 +974,16 @@
       <c r="A14">
         <v>1715721</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>3</v>
       </c>
       <c r="F14">
@@ -978,16 +998,16 @@
       <c r="A15">
         <v>1988846</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>2</v>
       </c>
       <c r="F15">
@@ -1002,16 +1022,16 @@
       <c r="A16">
         <v>1988998</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>2</v>
       </c>
       <c r="F16">
@@ -1026,16 +1046,16 @@
       <c r="A17">
         <v>1770979</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>1</v>
       </c>
       <c r="F17">
@@ -1050,16 +1070,16 @@
       <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18">
@@ -1074,16 +1094,16 @@
       <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>1</v>
       </c>
       <c r="F19">
@@ -1095,19 +1115,19 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>1</v>
       </c>
       <c r="F20">
@@ -1119,19 +1139,19 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>1</v>
       </c>
       <c r="F21">
@@ -1143,22 +1163,22 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>2</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>0.01</v>
       </c>
       <c r="G22">
@@ -1167,22 +1187,22 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <v>9.8200000000000006E-3</v>
       </c>
       <c r="G23">
@@ -1191,19 +1211,19 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>1</v>
       </c>
       <c r="F24">
@@ -1215,22 +1235,22 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>1</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="3">
         <v>7.3600000000000002E-3</v>
       </c>
       <c r="G25">
@@ -1239,22 +1259,22 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="1">
         <v>1</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="3">
         <v>9.8200000000000006E-3</v>
       </c>
       <c r="G26">
@@ -1263,22 +1283,22 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="1">
         <v>10</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="3">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="G27">
@@ -1287,22 +1307,22 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>4</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="3">
         <v>5.4359999999999999E-2</v>
       </c>
       <c r="G28">
@@ -1310,47 +1330,47 @@
         <v>0.21743999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:7" ht="16" customHeight="1">
+      <c r="A29" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3">
+        <v>16.920000000000002</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>16.920000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16" customHeight="1">
+      <c r="A30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29" s="4">
-        <v>0.92</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>2</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="3">
         <v>5.3969999999999997E-2</v>
       </c>
       <c r="G30">
@@ -1359,19 +1379,19 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>744772390</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="2">
+      <c r="C31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="1">
         <v>1</v>
       </c>
       <c r="F31">
@@ -1383,24 +1403,32 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="B32" s="7" t="s">
+      <c r="A32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="2">
+      <c r="E32" s="1">
         <v>2</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="3">
         <v>2.11</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
         <v>4.22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="31">
+      <c r="A33" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added connectors to BOM and changed the battery input label
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard.xlsx
+++ b/BOM/BOM_PowerBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9623EC4D-FA9D-C646-80A9-810BC201ED7B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1FB65B-E9F5-F548-90A6-64ECF16C871F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14060" yWindow="460" windowWidth="10080" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
+    <workbookView xWindow="7660" yWindow="460" windowWidth="17940" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>Manufacturer Number</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>300V 10A 6-Position Terminal Block</t>
-  </si>
-  <si>
-    <t>150V 5A 4-Position</t>
   </si>
   <si>
     <t>10118194-0001LF</t>
@@ -258,6 +255,12 @@
   </si>
   <si>
     <t>5 mOhm 18W Resistor</t>
+  </si>
+  <si>
+    <t>600V 101A 2-position Vertical Terminal Block</t>
+  </si>
+  <si>
+    <t>150V 17.5A 4-Position Vertical Terminal Block</t>
   </si>
 </sst>
 </file>
@@ -331,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -346,6 +349,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DE3487-35ED-9947-B91A-5715036B4C63}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -671,16 +677,16 @@
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1">
-        <f>SUM(G3:G192)</f>
-        <v>109.07638000000001</v>
+        <f>SUM(G3:G193)</f>
+        <v>107.68638000000001</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -703,7 +709,7 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -716,7 +722,7 @@
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="1">
@@ -740,7 +746,7 @@
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="1">
@@ -750,7 +756,7 @@
         <v>2E-3</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G32" si="0">E4*F4</f>
+        <f t="shared" ref="G4:G33" si="0">E4*F4</f>
         <v>2.6000000000000002E-2</v>
       </c>
     </row>
@@ -764,7 +770,7 @@
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1">
@@ -788,7 +794,7 @@
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1">
@@ -812,7 +818,7 @@
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="1">
@@ -836,7 +842,7 @@
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="1">
@@ -860,7 +866,7 @@
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="1">
@@ -884,7 +890,7 @@
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="1">
@@ -908,7 +914,7 @@
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="1">
@@ -932,7 +938,7 @@
       <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E12" s="1">
@@ -956,23 +962,23 @@
       <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="10" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>8.68</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="32">
       <c r="A14">
-        <v>1715721</v>
+        <v>1845344</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>32</v>
@@ -980,47 +986,47 @@
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>34</v>
+      <c r="D14" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="E14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>1.27</v>
+        <v>15.5</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>3.81</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>1988846</v>
+        <v>1715721</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="E15" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15">
-        <v>1.1599999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>2.3199999999999998</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>1988998</v>
+        <v>1988846</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>32</v>
@@ -1028,128 +1034,128 @@
       <c r="C16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>36</v>
+      <c r="D16" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
       <c r="F16">
-        <v>1.28</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>2.56</v>
+        <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>1770979</v>
+        <v>1988998</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="E17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>0.86</v>
+        <v>1.28</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>38</v>
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="32">
+      <c r="A18" s="4">
+        <v>1984785</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
+      <c r="D18" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18">
-        <v>0.42</v>
+        <v>1.33</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>0.42</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0.42</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>7.02</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>7.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17">
+      <c r="A21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>7.02</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>7.02</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="17">
-      <c r="A20" s="4" t="s">
+      <c r="C21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>5</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -1162,33 +1168,33 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="32">
       <c r="A22" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>57</v>
+      <c r="D22" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E22" s="1">
-        <v>2</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0.01</v>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>19</v>
@@ -1196,23 +1202,23 @@
       <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>58</v>
+      <c r="D23" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="E23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" s="3">
-        <v>9.8200000000000006E-3</v>
+        <v>0.01</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>9.8200000000000006E-3</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>19</v>
@@ -1220,18 +1226,18 @@
       <c r="C24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>59</v>
+      <c r="D24" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
       </c>
-      <c r="F24">
-        <v>0.01</v>
+      <c r="F24" s="3">
+        <v>9.8200000000000006E-3</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>9.8200000000000006E-3</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1244,71 +1250,71 @@
       <c r="C25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>60</v>
+      <c r="D25" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
       </c>
-      <c r="F25" s="3">
-        <v>7.3600000000000002E-3</v>
+      <c r="F25">
+        <v>0.01</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>7.3600000000000002E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>61</v>
+        <v>15</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
       </c>
       <c r="F26" s="3">
-        <v>9.8200000000000006E-3</v>
+        <v>7.3600000000000002E-3</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>9.8200000000000006E-3</v>
+        <v>7.3600000000000002E-3</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>56</v>
+        <v>30</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="E27" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3">
-        <v>3.6999999999999998E-2</v>
+        <v>9.8200000000000006E-3</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>0.37</v>
+        <v>9.8200000000000006E-3</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>19</v>
@@ -1316,119 +1322,143 @@
       <c r="C28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="1">
+        <v>10</v>
+      </c>
+      <c r="F28" s="3">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="1">
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="1">
         <v>4</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F29" s="3">
         <v>5.4359999999999999E-2</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <f t="shared" si="0"/>
         <v>0.21743999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16" customHeight="1">
-      <c r="A29" s="7" t="s">
+    <row r="30" spans="1:7" ht="16" customHeight="1">
+      <c r="A30" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="1">
-        <v>1</v>
-      </c>
-      <c r="F29" s="3">
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
         <v>16.920000000000002</v>
       </c>
-      <c r="G29">
+      <c r="G30">
         <f t="shared" si="0"/>
         <v>16.920000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16" customHeight="1">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:7" ht="16" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="E31" s="1">
         <v>2</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F31" s="3">
         <v>5.3969999999999997E-2</v>
       </c>
-      <c r="G30">
+      <c r="G31">
         <f t="shared" si="0"/>
         <v>0.10793999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="3">
+    <row r="32" spans="1:7">
+      <c r="A32" s="3">
         <v>744772390</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1.37</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="32">
+      <c r="A33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="1">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>1.37</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="0"/>
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="3" t="s">
+      <c r="C33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2</v>
+      </c>
+      <c r="F33" s="3">
+        <v>2.11</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="32">
+      <c r="A34" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="1">
-        <v>2</v>
-      </c>
-      <c r="F32" s="3">
-        <v>2.11</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="0"/>
-        <v>4.22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="32">
-      <c r="A33" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added labels for all components
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard.xlsx
+++ b/BOM/BOM_PowerBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1FB65B-E9F5-F548-90A6-64ECF16C871F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCB9ED7-A90E-AA4A-935C-36D7366108FF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7660" yWindow="460" windowWidth="17940" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
+    <workbookView xWindow="11580" yWindow="460" windowWidth="17940" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="81">
   <si>
     <t>Manufacturer Number</t>
   </si>
@@ -39,24 +39,12 @@
     <t>Price</t>
   </si>
   <si>
-    <t xml:space="preserve">HMK325 C7475[]N-TE </t>
-  </si>
-  <si>
     <t>100V 4.7uF Capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">HMK432 B7105[]M-T </t>
-  </si>
-  <si>
     <t>100V 1uF Capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">HMK107 B7104[]A-T </t>
-  </si>
-  <si>
-    <t>100V 0.1uF Capacitor</t>
-  </si>
-  <si>
     <t xml:space="preserve">TAIYO YUDEN </t>
   </si>
   <si>
@@ -66,9 +54,6 @@
     <t>100V 10nF Capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">UMK105 BJ103[]V-F </t>
-  </si>
-  <si>
     <t>Supplier</t>
   </si>
   <si>
@@ -174,52 +159,16 @@
     <t>Microchip Technology</t>
   </si>
   <si>
-    <t>ERJ-1GEF1004C</t>
-  </si>
-  <si>
-    <t>ERJ-1GEJ303C</t>
-  </si>
-  <si>
-    <t>ERJ-1GEF2002C</t>
-  </si>
-  <si>
-    <t>ERJ-1GEF3003C</t>
-  </si>
-  <si>
-    <t>ERJ-1GEF1002C</t>
-  </si>
-  <si>
     <t>ERJ-PB3B1001V</t>
   </si>
   <si>
     <t>1k Ohm 0.2W Resistor</t>
   </si>
   <si>
-    <t>1M ohm 0.02W resistor</t>
-  </si>
-  <si>
-    <t>10k ohm 0.05Wresistor</t>
-  </si>
-  <si>
-    <t>20k Ohm 0.05W Resistor</t>
-  </si>
-  <si>
-    <t>30k Ohm 0.05W Resistor</t>
-  </si>
-  <si>
-    <t>300k Ohm 0.05W Resistor</t>
-  </si>
-  <si>
     <t>100 Ohm 0.1W Resistor</t>
   </si>
   <si>
     <t>ERA-3AEB101V</t>
-  </si>
-  <si>
-    <t>ERJ-MP3KF5M0U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10k Ohm Thermistor </t>
   </si>
   <si>
     <t>Total per Part</t>
@@ -261,13 +210,73 @@
   </si>
   <si>
     <t>150V 17.5A 4-Position Vertical Terminal Block</t>
+  </si>
+  <si>
+    <t>CPF0603B1M0E1</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>1M ohm 0.02W resistor 0603</t>
+  </si>
+  <si>
+    <t>ERA-3AEB103V</t>
+  </si>
+  <si>
+    <t>10k ohm 0.05Wresistor 0603</t>
+  </si>
+  <si>
+    <t>ERA-3AEB203V</t>
+  </si>
+  <si>
+    <t>20k Ohm 0.1W Resistor 0603</t>
+  </si>
+  <si>
+    <t>ERA-3AEB303V</t>
+  </si>
+  <si>
+    <t>ERA-3AEB304V</t>
+  </si>
+  <si>
+    <t>30k Ohm 0.1W Resistor 0603</t>
+  </si>
+  <si>
+    <t>300k Ohm 0.1W Resistor 0603</t>
+  </si>
+  <si>
+    <t>GCM188R72A103KA37D</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMK325 C7475KN-TE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMK432 B7105KM-T </t>
+  </si>
+  <si>
+    <t>CC0603KRX7R0BB104</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>100V 0.1uF Capacitor 0603</t>
+  </si>
+  <si>
+    <t>ERT-J1VR103J</t>
+  </si>
+  <si>
+    <t>10k Ohm Thermistor 0603</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -308,11 +317,6 @@
       <color theme="1"/>
       <name val="HelveticaLTStd"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="MS"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -334,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -348,7 +352,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -668,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DE3487-35ED-9947-B91A-5715036B4C63}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -682,11 +685,11 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B1">
         <f>SUM(G3:G193)</f>
-        <v>107.68638000000001</v>
+        <v>109.92937999999998</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -694,10 +697,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -709,21 +712,21 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>5</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -738,16 +741,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="E4" s="1">
         <v>13</v>
@@ -762,16 +765,16 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
@@ -785,17 +788,17 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="9" t="s">
-        <v>13</v>
+      <c r="A6" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -810,16 +813,16 @@
     </row>
     <row r="7" spans="1:7" ht="17">
       <c r="A7" s="8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E7" s="1">
         <v>18</v>
@@ -834,16 +837,16 @@
     </row>
     <row r="8" spans="1:7" ht="17">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -858,16 +861,16 @@
     </row>
     <row r="9" spans="1:7" ht="17">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="E9" s="1">
         <v>3</v>
@@ -882,16 +885,16 @@
     </row>
     <row r="10" spans="1:7" ht="17">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -906,16 +909,16 @@
     </row>
     <row r="11" spans="1:7" ht="17">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -930,16 +933,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
@@ -957,13 +960,13 @@
         <v>1770539</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>33</v>
+        <v>10</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -981,13 +984,13 @@
         <v>1845344</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>76</v>
+        <v>10</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -1005,13 +1008,13 @@
         <v>1715721</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="E15" s="1">
         <v>3</v>
@@ -1029,13 +1032,13 @@
         <v>1988846</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>35</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
@@ -1053,13 +1056,13 @@
         <v>1988998</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -1077,13 +1080,13 @@
         <v>1984785</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>77</v>
+        <v>10</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -1098,16 +1101,16 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>39</v>
+        <v>10</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -1122,16 +1125,16 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>42</v>
+        <v>25</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -1146,16 +1149,16 @@
     </row>
     <row r="21" spans="1:7" ht="17">
       <c r="A21" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>45</v>
+        <v>12</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -1170,16 +1173,16 @@
     </row>
     <row r="22" spans="1:7" ht="32">
       <c r="A22" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -1194,136 +1197,136 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>56</v>
+        <v>10</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="E23" s="1">
         <v>2</v>
       </c>
       <c r="F23" s="3">
-        <v>0.01</v>
+        <v>0.44</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>57</v>
+        <v>10</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
       </c>
       <c r="F24" s="3">
-        <v>9.8200000000000006E-3</v>
+        <v>0.37</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>9.8200000000000006E-3</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>58</v>
+        <v>10</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
       </c>
       <c r="F25">
-        <v>0.01</v>
+        <v>0.35</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>59</v>
+        <v>10</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
       </c>
       <c r="F26" s="3">
-        <v>7.3600000000000002E-3</v>
+        <v>0.35</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>7.3600000000000002E-3</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>60</v>
+        <v>25</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
       </c>
       <c r="F27" s="3">
-        <v>9.8200000000000006E-3</v>
+        <v>0.35</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>9.8200000000000006E-3</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>55</v>
+        <v>10</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="E28" s="1">
         <v>10</v>
@@ -1338,16 +1341,16 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>61</v>
+        <v>10</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="E29" s="1">
         <v>4</v>
@@ -1362,16 +1365,16 @@
     </row>
     <row r="30" spans="1:7" ht="16" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>75</v>
+        <v>10</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -1386,16 +1389,16 @@
     </row>
     <row r="31" spans="1:7" ht="16" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>64</v>
+        <v>10</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="E31" s="1">
         <v>2</v>
@@ -1413,13 +1416,13 @@
         <v>744772390</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>67</v>
+        <v>10</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
@@ -1434,16 +1437,16 @@
     </row>
     <row r="33" spans="1:7" ht="32">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>70</v>
+        <v>10</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="E33" s="1">
         <v>2</v>
@@ -1458,7 +1461,7 @@
     </row>
     <row r="34" spans="1:7" ht="32">
       <c r="A34" s="6" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted capacitor prices a bit
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard.xlsx
+++ b/BOM/BOM_PowerBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCB9ED7-A90E-AA4A-935C-36D7366108FF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{43684280-FD66-3141-93D3-74BDFE5694E6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="460" windowWidth="17940" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
+    <workbookView xWindow="11580" yWindow="460" windowWidth="23680" windowHeight="23300" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DE3487-35ED-9947-B91A-5715036B4C63}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -689,7 +689,7 @@
       </c>
       <c r="B1">
         <f>SUM(G3:G193)</f>
-        <v>109.92937999999998</v>
+        <v>115.88937999999997</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -732,11 +732,11 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>2E-3</v>
+        <v>0.3</v>
       </c>
       <c r="G3">
         <f>E3*F3</f>
-        <v>4.0000000000000001E-3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -756,11 +756,11 @@
         <v>13</v>
       </c>
       <c r="F4">
-        <v>2E-3</v>
+        <v>0.3</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G33" si="0">E4*F4</f>
-        <v>2.6000000000000002E-2</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -780,11 +780,11 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>2E-3</v>
+        <v>0.3</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>6.0000000000000001E-3</v>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -804,11 +804,11 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>2E-3</v>
+        <v>0.3</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>4.0000000000000001E-3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17">

</xml_diff>

<commit_message>
Updated prices & amounts for components in powerboard BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard.xlsx
+++ b/BOM/BOM_PowerBoard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyrel\rover-hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{43684280-FD66-3141-93D3-74BDFE5694E6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE275FC-CCD5-4598-8700-9F02CC7D621B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="460" windowWidth="23680" windowHeight="23300" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
+    <workbookView xWindow="11580" yWindow="465" windowWidth="23685" windowHeight="23295" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,30 +39,18 @@
     <t>Price</t>
   </si>
   <si>
-    <t>100V 4.7uF Capacitor</t>
-  </si>
-  <si>
-    <t>100V 1uF Capacitor</t>
-  </si>
-  <si>
     <t xml:space="preserve">TAIYO YUDEN </t>
   </si>
   <si>
     <t>Manufacturer</t>
   </si>
   <si>
-    <t>100V 10nF Capacitor</t>
-  </si>
-  <si>
     <t>Supplier</t>
   </si>
   <si>
     <t>Digikey</t>
   </si>
   <si>
-    <t>EEUFS1H681( )</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
@@ -90,24 +78,9 @@
     <t>35V 68uF Capacitor</t>
   </si>
   <si>
-    <t>Taiwan Semiconductor</t>
-  </si>
-  <si>
-    <t>TSZU52C9V1 RG</t>
-  </si>
-  <si>
-    <t>9.1V 150mW Zener Diode</t>
-  </si>
-  <si>
-    <t>RB751V-40WS RRG</t>
-  </si>
-  <si>
     <t>digikey</t>
   </si>
   <si>
-    <t>40V 30mA Diode</t>
-  </si>
-  <si>
     <t>Phoenix Contact</t>
   </si>
   <si>
@@ -160,9 +133,6 @@
   </si>
   <si>
     <t>ERJ-PB3B1001V</t>
-  </si>
-  <si>
-    <t>1k Ohm 0.2W Resistor</t>
   </si>
   <si>
     <t>100 Ohm 0.1W Resistor</t>
@@ -196,10 +166,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-MP2060-0.005J-ND </t>
-  </si>
-  <si>
     <t>Caddock Electronics Inc.</t>
   </si>
   <si>
@@ -251,18 +217,6 @@
     <t>Murata Electronics</t>
   </si>
   <si>
-    <t xml:space="preserve">HMK325 C7475KN-TE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HMK432 B7105KM-T </t>
-  </si>
-  <si>
-    <t>CC0603KRX7R0BB104</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
     <t>100V 0.1uF Capacitor 0603</t>
   </si>
   <si>
@@ -270,13 +224,58 @@
   </si>
   <si>
     <t>10k Ohm Thermistor 0603</t>
+  </si>
+  <si>
+    <t>HMK325C7475KN-TE</t>
+  </si>
+  <si>
+    <t>100V 4.7uF Capacitor 1210</t>
+  </si>
+  <si>
+    <t>HMK432 B7105KM-T</t>
+  </si>
+  <si>
+    <t>C1608X7S2A104M080AB</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>100V 1uF Capacitor 1210</t>
+  </si>
+  <si>
+    <t>100V 10nF Capacitor 0603</t>
+  </si>
+  <si>
+    <t>EEU-FS1H681B</t>
+  </si>
+  <si>
+    <t>DZ2S091M0L</t>
+  </si>
+  <si>
+    <t>9.1V 150mW Zener Diode 0603</t>
+  </si>
+  <si>
+    <t>SD0603S040S0R2</t>
+  </si>
+  <si>
+    <t>AVX Corporation</t>
+  </si>
+  <si>
+    <t>40V 200mA Diode</t>
+  </si>
+  <si>
+    <t>1k Ohm 0.2W Resistor 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP2060-0.005J-ND </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -317,13 +316,26 @@
       <color theme="1"/>
       <name val="HelveticaLTStd"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -338,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -354,6 +366,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -669,38 +686,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DE3487-35ED-9947-B91A-5715036B4C63}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="1" max="1" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.625" customWidth="1"/>
+    <col min="4" max="4" width="32.125" customWidth="1"/>
+    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B1">
         <f>SUM(G3:G193)</f>
-        <v>115.88937999999997</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>140.56799999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -712,141 +730,146 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
       </c>
       <c r="F3">
-        <v>0.3</v>
+        <v>1.99</v>
       </c>
       <c r="G3">
         <f>E3*F3</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>3.98</v>
+      </c>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1">
         <v>13</v>
       </c>
       <c r="F4">
-        <v>0.3</v>
+        <v>1.0820000000000001</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G33" si="0">E4*F4</f>
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>14.066000000000001</v>
+      </c>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>0.3</v>
+        <v>0.26700000000000002</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>8</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
       </c>
       <c r="F6">
-        <v>0.3</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="17">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" ht="16.5">
       <c r="A7" s="8" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1">
         <v>18</v>
       </c>
       <c r="F7">
-        <v>1.6</v>
+        <v>1.5049999999999999</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>28.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17">
+        <v>27.089999999999996</v>
+      </c>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" ht="16.5">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -858,115 +881,117 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="17">
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" ht="16.5">
       <c r="A9" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="E9" s="1">
         <v>3</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="17">
+        <v>1.3800000000000001</v>
+      </c>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" ht="16.5">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="17">
+        <v>0.75</v>
+      </c>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.5">
       <c r="A11" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>4.3999999999999997E-2</v>
+        <v>0.307</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>0.307</v>
+      </c>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
       </c>
       <c r="F12">
-        <v>0.3</v>
+        <v>0.64</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>1770539</v>
-      </c>
+        <v>1.92</v>
+      </c>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -978,163 +1003,170 @@
         <f t="shared" si="0"/>
         <v>8.68</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="32">
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" ht="31.5">
       <c r="A14">
         <v>1845344</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
       </c>
       <c r="F14">
-        <v>15.5</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>1715721</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E15" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>1.27</v>
+        <v>1.77</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>3.81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>1.77</v>
+      </c>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>1988846</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E16" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <v>1.1599999999999999</v>
+        <v>1.61</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>2.3199999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>4.83</v>
+      </c>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>1988998</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
       </c>
       <c r="F17">
-        <v>1.28</v>
+        <v>1.78</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="32">
+        <v>3.56</v>
+      </c>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="1:8" ht="31.5">
       <c r="A18" s="4">
         <v>1984785</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>2.27</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>2.27</v>
+      </c>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1.33</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="0"/>
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>0.42</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -1146,322 +1178,336 @@
         <f t="shared" si="0"/>
         <v>7.02</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="17">
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" ht="16.5">
       <c r="A21" s="4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>5.22</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="32">
+        <v>5.22</v>
+      </c>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" ht="31.5">
       <c r="A22" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
       </c>
       <c r="F22">
-        <v>5</v>
+        <v>4.7699999999999996</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E23" s="1">
         <v>2</v>
       </c>
       <c r="F23" s="3">
-        <v>0.44</v>
+        <v>0.65</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>1.3</v>
+      </c>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.37</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0.52</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>0.35</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0.35</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
       </c>
       <c r="F27" s="3">
-        <v>0.35</v>
+        <v>0.52</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>0.52</v>
+      </c>
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="E28" s="1">
         <v>10</v>
       </c>
       <c r="F28" s="3">
-        <v>3.6999999999999998E-2</v>
+        <v>0.22</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E29" s="1">
         <v>4</v>
       </c>
       <c r="F29" s="3">
-        <v>5.4359999999999999E-2</v>
+        <v>0.44</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>0.21743999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="16" customHeight="1">
+        <v>1.76</v>
+      </c>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.95" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
+        <v>17.149999999999999</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>17.149999999999999</v>
+      </c>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.95" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="3">
-        <v>16.920000000000002</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="0"/>
-        <v>16.920000000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="16" customHeight="1">
-      <c r="A31" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C31" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="E31" s="1">
         <v>2</v>
       </c>
       <c r="F31" s="3">
-        <v>5.3969999999999997E-2</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
-        <v>0.10793999999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="3">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="12">
         <v>744772390</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
       </c>
       <c r="F32">
-        <v>1.37</v>
+        <v>1.34</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="32">
+        <v>1.34</v>
+      </c>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E33" s="1">
         <v>2</v>
       </c>
       <c r="F33" s="3">
-        <v>2.11</v>
+        <v>1.86</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
-        <v>4.22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="32">
+        <v>3.72</v>
+      </c>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" ht="31.5">
       <c r="A34" s="6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arm power board v2
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard.xlsx
+++ b/BOM/BOM_PowerBoard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyrel\rover-hardware\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5BE80B-C7B2-43F6-B147-5D0997DDB35D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53182B89-67EC-544B-9CC6-13C991538789}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="465" windowWidth="23685" windowHeight="23295" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
+    <workbookView xWindow="1920" yWindow="460" windowWidth="23680" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
   <si>
     <t>Manufacturer Number</t>
   </si>
@@ -147,10 +147,6 @@
     <t xml:space="preserve">IRF3205PBF </t>
   </si>
   <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
     <t>Caddock Electronics Inc.</t>
   </si>
   <si>
@@ -293,13 +289,31 @@
   </si>
   <si>
     <t>50V 0.1uF Capacitor 0603</t>
+  </si>
+  <si>
+    <t>DMP3099L-7</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>digikey</t>
+  </si>
+  <si>
+    <t>P-Channel 30V 3.8A (Ta) 1.08W (Ta) Surface Mount SOT-23</t>
+  </si>
+  <si>
+    <t>BSS138CT-ND</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 50V 220mA SOT-23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -341,6 +355,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -393,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -423,6 +443,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,36 +758,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DE3487-35ED-9947-B91A-5715036B4C63}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.625" customWidth="1"/>
-    <col min="4" max="4" width="38.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="16">
         <f>SUM(G3:G193)</f>
-        <v>161.60700000000003</v>
+        <v>163.09700000000004</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,9 +810,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>4</v>
@@ -800,7 +821,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="10">
         <v>2</v>
@@ -814,9 +835,9 @@
       </c>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>4</v>
@@ -825,7 +846,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" s="10">
         <v>13</v>
@@ -839,18 +860,18 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>86</v>
-      </c>
       <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="10">
         <v>3</v>
@@ -864,19 +885,19 @@
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="10">
         <v>2</v>
@@ -890,9 +911,9 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>10</v>
@@ -915,7 +936,7 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
@@ -940,10 +961,10 @@
       </c>
       <c r="H8" s="6"/>
       <c r="J8" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>11</v>
       </c>
@@ -969,10 +990,10 @@
       <c r="H9" s="6"/>
       <c r="J9" s="2"/>
       <c r="K9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
@@ -998,12 +1019,12 @@
       <c r="H10" s="6"/>
       <c r="J10" s="8"/>
       <c r="K10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>10</v>
@@ -1012,7 +1033,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11" s="10">
         <v>1</v>
@@ -1027,21 +1048,21 @@
       <c r="H11" s="9"/>
       <c r="J11" s="3"/>
       <c r="K11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>64</v>
-      </c>
       <c r="C12" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="10">
         <v>3</v>
@@ -1056,10 +1077,10 @@
       <c r="H12" s="6"/>
       <c r="J12" s="4"/>
       <c r="K12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="15" t="s">
         <v>17</v>
@@ -1068,7 +1089,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E13" s="10">
         <v>1</v>
@@ -1082,7 +1103,7 @@
       </c>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>1845344</v>
       </c>
@@ -1093,7 +1114,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E14" s="10">
         <v>1</v>
@@ -1107,7 +1128,7 @@
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>1715721</v>
       </c>
@@ -1118,7 +1139,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="10">
         <v>1</v>
@@ -1132,7 +1153,7 @@
       </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>1715190</v>
       </c>
@@ -1143,7 +1164,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E16" s="10">
         <v>4</v>
@@ -1157,7 +1178,7 @@
       </c>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>1988846</v>
       </c>
@@ -1168,7 +1189,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E17" s="10">
         <v>4</v>
@@ -1177,14 +1198,14 @@
         <v>1.61</v>
       </c>
       <c r="G17" s="10">
-        <f>E17*F17</f>
+        <f t="shared" ref="G17:G36" si="1">E17*F17</f>
         <v>6.44</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>1988998</v>
       </c>
@@ -1195,7 +1216,7 @@
         <v>7</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18" s="10">
         <v>2</v>
@@ -1204,14 +1225,14 @@
         <v>1.78</v>
       </c>
       <c r="G18" s="10">
-        <f>E18*F18</f>
+        <f t="shared" si="1"/>
         <v>3.56</v>
       </c>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>17</v>
@@ -1220,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19" s="10">
         <v>1</v>
@@ -1229,12 +1250,12 @@
         <v>2.27</v>
       </c>
       <c r="G19" s="10">
-        <f>E19*F19</f>
+        <f t="shared" si="1"/>
         <v>2.27</v>
       </c>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>18</v>
       </c>
@@ -1254,12 +1275,12 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="G20" s="10">
-        <f>E20*F20</f>
+        <f t="shared" si="1"/>
         <v>0.57999999999999996</v>
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>21</v>
       </c>
@@ -1279,12 +1300,12 @@
         <v>7.02</v>
       </c>
       <c r="G21" s="10">
-        <f>E21*F21</f>
+        <f t="shared" si="1"/>
         <v>7.02</v>
       </c>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>25</v>
       </c>
@@ -1304,12 +1325,12 @@
         <v>5.22</v>
       </c>
       <c r="G22" s="10">
-        <f>E22*F22</f>
+        <f t="shared" si="1"/>
         <v>5.22</v>
       </c>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -1329,23 +1350,23 @@
         <v>4.7699999999999996</v>
       </c>
       <c r="G23" s="10">
-        <f>E23*F23</f>
+        <f t="shared" si="1"/>
         <v>4.7699999999999996</v>
       </c>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="C24" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="E24" s="10">
         <v>2</v>
@@ -1354,14 +1375,14 @@
         <v>0.65</v>
       </c>
       <c r="G24" s="10">
-        <f>E24*F24</f>
+        <f t="shared" si="1"/>
         <v>1.3</v>
       </c>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>10</v>
@@ -1370,7 +1391,7 @@
         <v>7</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E25" s="10">
         <v>1</v>
@@ -1379,14 +1400,14 @@
         <v>0.52</v>
       </c>
       <c r="G25" s="10">
-        <f>E25*F25</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>10</v>
@@ -1395,7 +1416,7 @@
         <v>7</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="10">
         <v>1</v>
@@ -1404,14 +1425,14 @@
         <v>0.52</v>
       </c>
       <c r="G26" s="10">
-        <f>E26*F26</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>10</v>
@@ -1420,7 +1441,7 @@
         <v>7</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E27" s="10">
         <v>1</v>
@@ -1429,14 +1450,14 @@
         <v>0.52</v>
       </c>
       <c r="G27" s="10">
-        <f>E27*F27</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>10</v>
@@ -1445,7 +1466,7 @@
         <v>7</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E28" s="10">
         <v>1</v>
@@ -1454,12 +1475,12 @@
         <v>0.52</v>
       </c>
       <c r="G28" s="10">
-        <f>E28*F28</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>30</v>
       </c>
@@ -1470,7 +1491,7 @@
         <v>7</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E29" s="10">
         <v>10</v>
@@ -1479,12 +1500,12 @@
         <v>0.22</v>
       </c>
       <c r="G29" s="10">
-        <f>E29*F29</f>
+        <f t="shared" si="1"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>32</v>
       </c>
@@ -1504,23 +1525,23 @@
         <v>0.44</v>
       </c>
       <c r="G30" s="10">
-        <f>E30*F30</f>
+        <f t="shared" si="1"/>
         <v>1.76</v>
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="E31" s="10">
         <v>1</v>
@@ -1529,14 +1550,14 @@
         <v>17.149999999999999</v>
       </c>
       <c r="G31" s="10">
-        <f>E31*F31</f>
+        <f t="shared" si="1"/>
         <v>17.149999999999999</v>
       </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>10</v>
@@ -1545,7 +1566,7 @@
         <v>7</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" s="10">
         <v>2</v>
@@ -1554,12 +1575,12 @@
         <v>0.32200000000000001</v>
       </c>
       <c r="G32" s="10">
-        <f>E32*F32</f>
+        <f t="shared" si="1"/>
         <v>0.64400000000000002</v>
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="12">
         <v>744772390</v>
       </c>
@@ -1579,12 +1600,12 @@
         <v>1.34</v>
       </c>
       <c r="G33" s="10">
-        <f>E33*F33</f>
+        <f t="shared" si="1"/>
         <v>1.34</v>
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>39</v>
       </c>
@@ -1604,21 +1625,58 @@
         <v>1.86</v>
       </c>
       <c r="G34" s="10">
-        <f>E34*F34</f>
+        <f t="shared" si="1"/>
         <v>3.72</v>
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1</v>
+      </c>
+      <c r="F35" s="10">
+        <v>0.61</v>
+      </c>
+      <c r="G35" s="10">
+        <f t="shared" si="1"/>
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="10">
+        <v>2</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0.44</v>
+      </c>
+      <c r="G36" s="10">
+        <f t="shared" si="1"/>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E37" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>